<commit_message>
Modified one data row of the sheet oneWayFlightSort
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/oneWayFlightSort.xlsx
+++ b/src/test/resources/datasheets/oneWayFlightSort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bajwauto\Projects\MultiAppPOM\multiApp\src\test\resources\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A95294-183F-4B07-B1EB-011A89E6CCD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B17F70-E5F7-49EE-86A0-01F5A29B795D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>

</xml_diff>